<commit_message>
fixed utility vs investor labeling
</commit_message>
<xml_diff>
--- a/generic token valuation model.xlsx
+++ b/generic token valuation model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4360" yWindow="-23540" windowWidth="33780" windowHeight="16560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Disclosures and license" sheetId="2" r:id="rId1"/>
@@ -1075,11 +1075,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="727235632"/>
-        <c:axId val="727254992"/>
+        <c:axId val="360993376"/>
+        <c:axId val="360995696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="727235632"/>
+        <c:axId val="360993376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1122,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="727254992"/>
+        <c:crossAx val="360995696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1130,7 +1130,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="727254992"/>
+        <c:axId val="360995696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,7 +1180,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="727235632"/>
+        <c:crossAx val="360993376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1326,7 +1326,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>% held by investors</c:v>
+                  <c:v>% used for utility</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1546,7 +1546,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>% used for utility</c:v>
+                  <c:v>% held by investors</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1766,11 +1766,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="642685248"/>
-        <c:axId val="642617472"/>
+        <c:axId val="361020944"/>
+        <c:axId val="361023264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="642685248"/>
+        <c:axId val="361020944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1813,7 +1813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="642617472"/>
+        <c:crossAx val="361023264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1821,7 +1821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="642617472"/>
+        <c:axId val="361023264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1872,7 +1872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="642685248"/>
+        <c:crossAx val="361020944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3112,16 +3112,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>927100</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3146,14 +3146,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3587,11 +3587,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6673,7 +6673,7 @@
     <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="64"/>
       <c r="B30" s="64" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
         <v>42</v>
@@ -6822,7 +6822,7 @@
     <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" s="64"/>
       <c r="B31" s="64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
         <v>42</v>

</xml_diff>